<commit_message>
sn: update senegal forms
</commit_message>
<xml_diff>
--- a/LF/PreTAS/Senegal/2022/jul 2022/sn_lf_pretas_2_partcipants_202207.xlsx
+++ b/LF/PreTAS/Senegal/2022/jul 2022/sn_lf_pretas_2_partcipants_202207.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="95">
   <si>
     <t>type</t>
   </si>
@@ -138,43 +138,19 @@
     <t>Le répondant a-t-il donné son consentement?</t>
   </si>
   <si>
-    <t>p_num</t>
-  </si>
-  <si>
-    <t>Enter the order number</t>
-  </si>
-  <si>
-    <t>Must be between 1 and 410</t>
-  </si>
-  <si>
-    <t>Numéro d'ordre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Doit être compris entre 1 et 410 </t>
-  </si>
-  <si>
-    <t>. &gt; 0 and . &lt;= 410</t>
-  </si>
-  <si>
-    <t>The value must be between 1 and 410</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La valeur doit être compris entre 1 et 410 </t>
+    <t>select_one sex_list</t>
+  </si>
+  <si>
+    <t>p_sex</t>
+  </si>
+  <si>
+    <t>Sex of respondent</t>
+  </si>
+  <si>
+    <t>Sexe du participant</t>
   </si>
   <si>
     <t>${p_consent} = 'Oui'</t>
-  </si>
-  <si>
-    <t>select_one sex_list</t>
-  </si>
-  <si>
-    <t>p_sex</t>
-  </si>
-  <si>
-    <t>Sex of respondent</t>
-  </si>
-  <si>
-    <t>Sexe du participant</t>
   </si>
   <si>
     <t>p_age_yrs</t>
@@ -1021,7 +997,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1058,9 +1034,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1418,14 +1391,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A11" sqref="$A11:$XFD11"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="$A7:$XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -1460,10 +1433,10 @@
       <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="22" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="11" t="s">
@@ -1510,29 +1483,29 @@
       <c r="D2" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="25" t="s">
+      <c r="G2" s="16"/>
+      <c r="H2" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
       <c r="M2" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
       <c r="P2" s="13"/>
     </row>
     <row r="3" s="3" customFormat="1" spans="1:16">
@@ -1546,21 +1519,21 @@
         <v>28</v>
       </c>
       <c r="D3" s="15"/>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="24"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
       <c r="M3" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
       <c r="P3" s="13"/>
     </row>
     <row r="4" s="3" customFormat="1" spans="1:16">
@@ -1574,12 +1547,12 @@
         <v>31</v>
       </c>
       <c r="D4" s="15"/>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="24"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
       <c r="I4" s="14"/>
       <c r="J4" s="14"/>
       <c r="K4" s="13"/>
@@ -1589,7 +1562,7 @@
       </c>
       <c r="N4" s="14"/>
       <c r="O4" s="14"/>
-      <c r="P4" s="17"/>
+      <c r="P4" s="16"/>
     </row>
     <row r="5" s="3" customFormat="1" spans="1:16">
       <c r="A5" s="13" t="s">
@@ -1602,12 +1575,12 @@
         <v>34</v>
       </c>
       <c r="D5" s="15"/>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="24"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
       <c r="K5" s="13"/>
@@ -1617,7 +1590,7 @@
       </c>
       <c r="N5" s="14"/>
       <c r="O5" s="14"/>
-      <c r="P5" s="17"/>
+      <c r="P5" s="16"/>
     </row>
     <row r="6" s="3" customFormat="1" spans="1:16">
       <c r="A6" s="13" t="s">
@@ -1630,12 +1603,12 @@
         <v>38</v>
       </c>
       <c r="D6" s="15"/>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="24"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="14"/>
-      <c r="H6" s="17"/>
+      <c r="H6" s="16"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
@@ -1647,67 +1620,63 @@
       <c r="O6" s="14"/>
       <c r="P6" s="14"/>
     </row>
-    <row r="7" s="3" customFormat="1" ht="28.5" spans="1:16">
-      <c r="A7" s="3" t="s">
+    <row r="7" s="3" customFormat="1" spans="1:16">
+      <c r="A7" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="23"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+    </row>
+    <row r="8" s="9" customFormat="1" ht="15.75" customHeight="1" spans="1:16">
+      <c r="A8" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="16" t="s">
+      <c r="B8" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="15"/>
+      <c r="E8" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="23"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="K8" s="14" t="s">
         <v>44</v>
-      </c>
-      <c r="G7" s="16"/>
-      <c r="H7" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="J7" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="L7" s="16"/>
-      <c r="M7" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="16"/>
-    </row>
-    <row r="8" s="3" customFormat="1" spans="1:16">
-      <c r="A8" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="F8" s="24"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="14" t="s">
-        <v>48</v>
       </c>
       <c r="L8" s="14"/>
       <c r="M8" s="14" t="s">
@@ -1717,153 +1686,139 @@
       <c r="O8" s="14"/>
       <c r="P8" s="14"/>
     </row>
-    <row r="9" s="9" customFormat="1" ht="15.75" customHeight="1" spans="1:16">
-      <c r="A9" s="17" t="s">
+    <row r="9" s="3" customFormat="1" ht="28.5" spans="1:16">
+      <c r="A9" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="F9" s="23"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="24" t="s">
+      <c r="I9" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="F9" s="24"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14" t="s">
+      <c r="J9" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="I9" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="J9" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="K9" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="L9" s="14"/>
+      <c r="K9" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="L9" s="16"/>
       <c r="M9" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-    </row>
-    <row r="10" s="3" customFormat="1" ht="28.5" spans="1:16">
-      <c r="A10" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="14" t="s">
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+    </row>
+    <row r="10" s="10" customFormat="1" ht="42.75" spans="1:16">
+      <c r="A10" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="19"/>
+      <c r="E10" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" s="15"/>
-      <c r="E10" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="F10" s="24"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="J10" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="K10" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="L10" s="17"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="L10" s="18"/>
       <c r="M10" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-    </row>
-    <row r="11" s="10" customFormat="1" ht="42.75" spans="1:16">
-      <c r="A11" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="19" t="s">
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" s="3" customFormat="1" ht="28.5" spans="1:16">
+      <c r="A11" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="19"/>
+      <c r="E11" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="25"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="L11" s="13"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+    </row>
+    <row r="12" s="3" customFormat="1" spans="1:16">
+      <c r="A12" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="B12" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="26" t="s">
+      <c r="C12" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="F11" s="26"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="L11" s="19"/>
-      <c r="M11" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" s="3" customFormat="1" ht="28.5" spans="1:16">
-      <c r="A12" s="13" t="s">
+      <c r="D12" s="19"/>
+      <c r="E12" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="F12" s="26"/>
+      <c r="F12" s="25"/>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
       <c r="J12" s="13"/>
-      <c r="K12" s="13" t="s">
-        <v>72</v>
-      </c>
+      <c r="K12" s="13"/>
       <c r="L12" s="13"/>
-      <c r="M12" s="14"/>
+      <c r="M12" s="13"/>
       <c r="N12" s="13"/>
       <c r="O12" s="13"/>
       <c r="P12" s="13"/>
     </row>
     <row r="13" s="3" customFormat="1" spans="1:16">
       <c r="A13" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="F13" s="26"/>
+        <v>69</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
@@ -1875,49 +1830,27 @@
       <c r="O13" s="13"/>
       <c r="P13" s="13"/>
     </row>
-    <row r="14" s="3" customFormat="1" spans="1:16">
+    <row r="14" spans="1:16">
       <c r="A14" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
+        <v>71</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
       <c r="E14" s="26"/>
       <c r="F14" s="26"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13"/>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="A15" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="21"/>
-      <c r="O15" s="21"/>
-      <c r="P15" s="21"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1947,7 +1880,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
@@ -1962,86 +1895,86 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="5" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="5" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="5" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="6" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="6" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2070,24 +2003,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>